<commit_message>
Updated to admin features
</commit_message>
<xml_diff>
--- a/assets/candidate-upload/contoh_db.xlsx
+++ b/assets/candidate-upload/contoh_db.xlsx
@@ -5,35 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilma\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop Presentasi 2\Desktop\New Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54626F70-28DA-4CBE-9144-BEB4D0FA2328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232332D7-016B-4945-B1C2-3A58AABC356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{FD5C508C-DDC2-4299-A4A8-4190B2D946F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ketentuan Upload" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
   <si>
     <t>Nama Lengkap</t>
   </si>
@@ -71,88 +64,277 @@
     <t>L</t>
   </si>
   <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>S-1</t>
-  </si>
-  <si>
-    <t>S-2</t>
-  </si>
-  <si>
-    <t>1997-11-5</t>
-  </si>
-  <si>
-    <t>1997-11-6</t>
-  </si>
-  <si>
-    <t>1997-11-7</t>
-  </si>
-  <si>
-    <t>1997-11-8</t>
-  </si>
-  <si>
-    <t>1997-11-9</t>
-  </si>
-  <si>
-    <t>1997-11-10</t>
-  </si>
-  <si>
-    <t>1997-11-11</t>
-  </si>
-  <si>
-    <t>1997-11-12</t>
-  </si>
-  <si>
-    <t>1997-11-13</t>
-  </si>
-  <si>
-    <t>1997-11-14</t>
-  </si>
-  <si>
-    <t>1997-11-15</t>
-  </si>
-  <si>
-    <t>1997-11-16</t>
-  </si>
-  <si>
-    <t>1997-11-17</t>
-  </si>
-  <si>
-    <t>1997-11-18</t>
-  </si>
-  <si>
-    <t>1997-11-19</t>
-  </si>
-  <si>
-    <t>1997-11-20</t>
-  </si>
-  <si>
-    <t>1997-11-21</t>
-  </si>
-  <si>
-    <t>1997-11-22</t>
-  </si>
-  <si>
-    <t>1997-11-23</t>
-  </si>
-  <si>
-    <t>1997-11-24</t>
-  </si>
-  <si>
-    <t>1997-11-25</t>
-  </si>
-  <si>
-    <t>D-3</t>
-  </si>
-  <si>
-    <t>D-2</t>
-  </si>
-  <si>
-    <t>D-4</t>
-  </si>
-  <si>
-    <t>D-1</t>
+    <t xml:space="preserve">Tanggal harus dalam bentuk format text (YYYY-MM-DD) </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Ketentuan</t>
+  </si>
+  <si>
+    <t>089528585858</t>
+  </si>
+  <si>
+    <t>Gunakan Kutip 1 (') di format nomor handphone</t>
+  </si>
+  <si>
+    <t>Tempat Lahir dalam bentuk text</t>
+  </si>
+  <si>
+    <t>Domisili dalam bentuk text</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin Laki-laki (L) , Perempuan (P) antara L/P</t>
+  </si>
+  <si>
+    <t>Gilang Ramadhan</t>
+  </si>
+  <si>
+    <t>Achirudin</t>
+  </si>
+  <si>
+    <t>Yusuf Maulana</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Jackline</t>
+  </si>
+  <si>
+    <t>Suci Rahmadani</t>
+  </si>
+  <si>
+    <t>Nurul Anisa</t>
+  </si>
+  <si>
+    <t>Abdi Basmallah</t>
+  </si>
+  <si>
+    <t>Siti Aisyah</t>
+  </si>
+  <si>
+    <t>Sugenda Anwar S.</t>
+  </si>
+  <si>
+    <t>Mustofah</t>
+  </si>
+  <si>
+    <t>Suci Dhea Friscila</t>
+  </si>
+  <si>
+    <t>Inggit Rizqiyah Nauli</t>
+  </si>
+  <si>
+    <t>Artha Uli Sitorus</t>
+  </si>
+  <si>
+    <t>Dara Anggraini</t>
+  </si>
+  <si>
+    <t>Siti Suherni</t>
+  </si>
+  <si>
+    <t>Octaviani</t>
+  </si>
+  <si>
+    <t>Risky Gunawan Trisnaardi</t>
+  </si>
+  <si>
+    <t>082314772222</t>
+  </si>
+  <si>
+    <t>082112611753</t>
+  </si>
+  <si>
+    <t>083893959764</t>
+  </si>
+  <si>
+    <t>081818200495</t>
+  </si>
+  <si>
+    <t>087873978695</t>
+  </si>
+  <si>
+    <t>082262534379</t>
+  </si>
+  <si>
+    <t>08987416186</t>
+  </si>
+  <si>
+    <t>082112389171</t>
+  </si>
+  <si>
+    <t>081280384908</t>
+  </si>
+  <si>
+    <t>087878691969</t>
+  </si>
+  <si>
+    <t>085692565477</t>
+  </si>
+  <si>
+    <t>081315000413</t>
+  </si>
+  <si>
+    <t>085774975116</t>
+  </si>
+  <si>
+    <t>087821487554</t>
+  </si>
+  <si>
+    <t>082297097870</t>
+  </si>
+  <si>
+    <t>089530320635</t>
+  </si>
+  <si>
+    <t>089610933279</t>
+  </si>
+  <si>
+    <t>089602696985</t>
+  </si>
+  <si>
+    <t>Klaten</t>
+  </si>
+  <si>
+    <t>Stabat</t>
+  </si>
+  <si>
+    <t>Pasar Gompong</t>
+  </si>
+  <si>
+    <t>Limas Jaya</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>Tanjungkarang</t>
+  </si>
+  <si>
+    <t>Jambi</t>
+  </si>
+  <si>
+    <t>Bekasi</t>
+  </si>
+  <si>
+    <t>Kebumen</t>
+  </si>
+  <si>
+    <t>Tangerang</t>
+  </si>
+  <si>
+    <t>Karawang</t>
+  </si>
+  <si>
+    <t>1995-03-04</t>
+  </si>
+  <si>
+    <t>1983-12-14</t>
+  </si>
+  <si>
+    <t>1987-01-25</t>
+  </si>
+  <si>
+    <t>1995-04-20</t>
+  </si>
+  <si>
+    <t>1998-10-20</t>
+  </si>
+  <si>
+    <t>1997-12-31</t>
+  </si>
+  <si>
+    <t>1996-06-16</t>
+  </si>
+  <si>
+    <t>1997-07-02</t>
+  </si>
+  <si>
+    <t>1995-12-13</t>
+  </si>
+  <si>
+    <t>1986-01-20</t>
+  </si>
+  <si>
+    <t>1985-06-20</t>
+  </si>
+  <si>
+    <t>1998-06-12</t>
+  </si>
+  <si>
+    <t>1996-09-12</t>
+  </si>
+  <si>
+    <t>1998-03-13</t>
+  </si>
+  <si>
+    <t>1997-08-06</t>
+  </si>
+  <si>
+    <t>2000-01-20</t>
+  </si>
+  <si>
+    <t>2000-10-07</t>
+  </si>
+  <si>
+    <t>1998-11-03</t>
+  </si>
+  <si>
+    <t>1997-11-05</t>
+  </si>
+  <si>
+    <t>Daan Mogot</t>
+  </si>
+  <si>
+    <t>Pasar Minggu</t>
+  </si>
+  <si>
+    <t>Ciputat</t>
+  </si>
+  <si>
+    <t>Cikarang</t>
+  </si>
+  <si>
+    <t>Karawaci</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>SMK</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Jagakarsa</t>
+  </si>
+  <si>
+    <t>Palmerah</t>
+  </si>
+  <si>
+    <t>Joglo</t>
+  </si>
+  <si>
+    <t>Duren Sawit</t>
+  </si>
+  <si>
+    <t>Cibitung</t>
+  </si>
+  <si>
+    <t>2022-10-20</t>
+  </si>
+  <si>
+    <t>Pendidikan text (D3) / (S1)</t>
   </si>
 </sst>
 </file>
@@ -202,10 +384,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -266,7 +449,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -318,7 +501,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -519,19 +702,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA1D44A-992C-460E-8A16-4DE32DF28325}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
@@ -567,316 +750,652 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>89528585858</v>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>27145456484</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>27145456484</v>
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>27145456484</v>
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>27145456484</v>
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>27145456484</v>
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>27145456484</v>
+        <v>25</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>27145456484</v>
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>27145456484</v>
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>27145456484</v>
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>27145456484</v>
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>27145456484</v>
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="94" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>